<commit_message>
Update auth login to support content type of query and x-www-form-urlencoded.
</commit_message>
<xml_diff>
--- a/doc/nacos-api.xlsx
+++ b/doc/nacos-api.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t>地址</t>
   </si>
@@ -144,6 +144,18 @@
   </si>
   <si>
     <t>/nacos/plugin-default-impl/nacos-default-auth-plugin/src/main/java/com/alibaba/nacos/plugin/auth/impl/controller/v3/UserControllerV3.java</t>
+  </si>
+  <si>
+    <t>IAuthenticationManager</t>
+  </si>
+  <si>
+    <t>/nacos/plugin-default-impl/nacos-default-auth-plugin/src/main/java/com/alibaba/nacos/plugin/auth/impl/authenticate/IAuthenticationManager.java</t>
+  </si>
+  <si>
+    <t>AbstractAuthenticationManager</t>
+  </si>
+  <si>
+    <t>/nacos/plugin-default-impl/nacos-default-auth-plugin/src/main/java/com/alibaba/nacos/plugin/auth/impl/authenticate/AbstractAuthenticationManager.java</t>
   </si>
 </sst>
 </file>
@@ -1314,12 +1326,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="20.4" outlineLevelCol="6"/>
@@ -1489,7 +1501,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" ht="102" spans="1:4">
+    <row r="14" ht="102" spans="1:6">
       <c r="A14" s="2" t="s">
         <v>35</v>
       </c>
@@ -1501,6 +1513,20 @@
       </c>
       <c r="D14" s="3" t="s">
         <v>38</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" ht="102" spans="5:6">
+      <c r="E15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>